<commit_message>
adding the POM,feature, extend report, utils file
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carfi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carfi\eclipse-workspace\API_Testing_Kata\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B0ADCF-7702-4A6F-BE3B-FB243D322938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8ECE4D-1501-46A5-8470-8B4CE64796E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,28 +44,6 @@
   </si>
   <si>
     <t>{
-        "firstname": "John",
-        "lastname": "Terry",
-        "totalprice": "2626",
-        "depositpaid": "true",
-            "checkin": "2021-02-23",
-            "checkout": "2021-10-23",
-        "additionalneeds": "Dinner"
-    }</t>
-  </si>
-  <si>
-    <t>{
-        "firstname": "Jim",
-        "lastname": "Brown",
-        "totalprice": "3200",
-        "depositpaid": "false",
-            "checkin": "2021-10-10",
-            "checkout": "2021-10-20",
-        "additionalneeds": "Breakfast"
-    }</t>
-  </si>
-  <si>
-    <t>{
   "roomid": 1,
   "firstname": "test",
   "lastname": "jo",
@@ -95,17 +73,60 @@
   <si>
     <t>https://automationintesting.online/api/booking</t>
   </si>
+  <si>
+    <t>{
+  "bookingid": 1,
+  "booking": {
+    "bookingid": 1,
+    "roomid": 1,
+    "firstname": "test",
+    "lastname": "jo",
+    "depositpaid": false,
+    "email": "test@test.com",
+    "phone": "314823489234",
+    "bookingdates": {
+      "checkin": "2025-08-13",
+      "checkout": "2025-08-14"
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  "bookingid": 2,
+  "booking": {
+    "bookingid": 2,
+    "roomid": 1,
+    "firstname": "test",
+    "lastname": "jonah",
+    "depositpaid": false,
+    "email": "test@test.com",
+    "phone": "314823489234",
+    "bookingdates": {
+      "checkin": "2025-08-23",
+      "checkout": "2025-08-24"
+    }
+  }
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -157,21 +178,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -455,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="15" customHeight="1"/>
@@ -491,13 +515,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="237.6" customHeight="1">
@@ -505,13 +529,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="237.6" customHeight="1">
@@ -528,7 +552,7 @@
     <row r="11" spans="1:5" ht="237.6" customHeight="1"/>
     <row r="12" spans="1:5" ht="237.6" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{30C9EE86-96C1-4F9B-83B9-BC7E898B226C}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
updating pom file, adding additional feature file and related step def
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carfi\eclipse-workspace\API_Testing_Kata\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8ECE4D-1501-46A5-8470-8B4CE64796E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5132326F-EDC8-42EF-B5EF-1CAF3F7C12FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>dataKey</t>
   </si>
@@ -109,12 +109,49 @@
   }
 }</t>
   </si>
+  <si>
+    <t>updateBooking1</t>
+  </si>
+  <si>
+    <t>{
+    "bookingid": 1,
+    "roomid": 1,
+    "firstname": "Jamestses1",
+    "lastname": "Dean1",
+    "depositpaid": true,
+    "bookingdates": {
+        "checkin": "2026-03-09",
+        "checkout": "2026-03-10"
+    }
+}</t>
+  </si>
+  <si>
+    <t>https://automationintesting.online/api/booking/id</t>
+  </si>
+  <si>
+    <t>{
+  "bookingid": 1,
+  "booking": {
+    "bookingid": 1,
+    "roomid": 1,
+    "firstname": "string",
+    "lastname": "string",
+    "depositpaid": true,
+    "email": "string",
+    "phone": "stringstrin",
+    "bookingdates": {
+      "checkin": "2026-03-09",
+        "checkout": "2026-03-10"
+    }
+  }
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +181,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -155,6 +199,12 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -178,25 +228,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -479,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="15" customHeight="1"/>
@@ -539,7 +595,18 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="237.6" customHeight="1">
-      <c r="B4" s="3"/>
+      <c r="A4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="237.6" customHeight="1">
       <c r="B5" s="3"/>
@@ -552,11 +619,12 @@
     <row r="11" spans="1:5" ht="237.6" customHeight="1"/>
     <row r="12" spans="1:5" ht="237.6" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{30C9EE86-96C1-4F9B-83B9-BC7E898B226C}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{80B50E66-0936-4C28-A92A-6D7566F7BD3B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>